<commit_message>
Fix missing value in test ARC Assay file
</commit_message>
<xml_diff>
--- a/tests/fixtures/testARC_proteomicsAlternativeTerms/assays/testAssayPRIDE/isa.assay.xlsx
+++ b/tests/fixtures/testARC_proteomicsAlternativeTerms/assays/testAssayPRIDE/isa.assay.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD8B3A7-718E-407B-A47A-AF02177BE53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A16040-7A37-4DC1-8A38-C60746A4A9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>ASSAY</t>
   </si>
@@ -654,7 +654,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,6 +760,9 @@
       <c r="D4" t="s">
         <v>30</v>
       </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
       <c r="F4" t="s">
         <v>32</v>
       </c>

</xml_diff>